<commit_message>
adapt main figure formatting of %
</commit_message>
<xml_diff>
--- a/Data/Experiment/Participants_2_12.xlsx
+++ b/Data/Experiment/Participants_2_12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\git\2025_Mueller_Hoener_Mann\Data\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529169F0-05ED-4708-AF3E-166C47A07B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EEDE5B-9D16-43BB-92CB-C63F83345FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6DE1AC28-3E97-4EA3-94F3-182769AE0F6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DE1AC28-3E97-4EA3-94F3-182769AE0F6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -230,27 +252,62 @@
     <t>Eliab</t>
   </si>
   <si>
-    <t>Yared</t>
-  </si>
-  <si>
     <t>Total valid:</t>
   </si>
   <si>
-    <t xml:space="preserve">Othman </t>
-  </si>
-  <si>
     <t>Daan Wensink</t>
   </si>
   <si>
     <t>Emiel</t>
+  </si>
+  <si>
+    <t>Patrick Ohallaran</t>
+  </si>
+  <si>
+    <t>2e klasse</t>
+  </si>
+  <si>
+    <t>Othman el Ghalbouri</t>
+  </si>
+  <si>
+    <t>Yared Koning</t>
+  </si>
+  <si>
+    <t>6e Klasse</t>
+  </si>
+  <si>
+    <t>1e divisie</t>
+  </si>
+  <si>
+    <t>4e Div</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>SD AGE</t>
+  </si>
+  <si>
+    <t>SD Years exp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -290,11 +347,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,20 +687,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B7697A-0658-480C-A7B0-8CEF981D0BC7}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
+    <col min="1" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -673,8 +731,11 @@
       <c r="K1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -705,8 +766,12 @@
       <c r="K2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="b">
+        <f>AND(J2=TRUE, K2=TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -737,8 +802,12 @@
       <c r="K3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="b">
+        <f t="shared" ref="L3:L27" si="0">AND(J3=TRUE, K3=TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -769,8 +838,12 @@
       <c r="K4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -801,8 +874,12 @@
       <c r="K5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -830,8 +907,12 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -859,8 +940,12 @@
       <c r="K7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -891,8 +976,12 @@
       <c r="K8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -923,8 +1012,12 @@
       <c r="K9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -952,8 +1045,12 @@
       <c r="K10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -981,8 +1078,12 @@
       <c r="K11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1010,8 +1111,12 @@
       <c r="K12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1042,8 +1147,12 @@
       <c r="K13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1071,8 +1180,12 @@
       <c r="K14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1100,8 +1213,12 @@
       <c r="K15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1118,6 +1235,9 @@
         <v>12</v>
       </c>
       <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
         <v>26</v>
       </c>
       <c r="J16" s="2" t="b">
@@ -1126,8 +1246,12 @@
       <c r="K16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1155,8 +1279,12 @@
       <c r="K17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1187,8 +1315,12 @@
       <c r="K18" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1219,8 +1351,12 @@
       <c r="K19" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1248,8 +1384,12 @@
       <c r="K20" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1280,84 +1420,250 @@
       <c r="K21" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22">
+        <v>24</v>
+      </c>
+      <c r="D22">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>70</v>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>65</v>
       </c>
-      <c r="J22" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s">
+        <v>58</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="J23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" t="b">
-        <v>1</v>
-      </c>
-      <c r="K24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="J25" t="b">
-        <v>1</v>
-      </c>
-      <c r="K25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="D27">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="4">
+        <f>AVERAGEIFS(C2:C27, J2:J27, "TRUE", K2:K27, "TRUE")</f>
+        <v>24.857142857142858</v>
+      </c>
+      <c r="D28" s="4">
+        <f>AVERAGEIFS(D2:D27, J2:J27, "TRUE", K2:K27, "TRUE")</f>
+        <v>18.952380952380953</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="J26" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J27" t="s">
-        <v>64</v>
-      </c>
-      <c r="K27">
-        <f>COUNTIFS(J2:J26,"=TRUE",K2:K26,"=TRUE")</f>
-        <v>20</v>
+      <c r="K28" s="4">
+        <f>COUNTIFS(J2:J27,"=TRUE",K2:K27,"=TRUE")</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="4" cm="1">
+        <f t="array" ref="C29">_xlfn.STDEV.S(_xlfn._xlws.FILTER(C2:C27, L2:L27=TRUE))</f>
+        <v>4.4976184174039782</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="4" cm="1">
+        <f t="array" ref="C30">_xlfn.STDEV.S(_xlfn._xlws.FILTER(D2:D27, L2:L27=TRUE))</f>
+        <v>3.7077781820949101</v>
       </c>
     </row>
   </sheetData>
@@ -1367,5 +1673,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>